<commit_message>
Update files for paper
</commit_message>
<xml_diff>
--- a/Datasets/homicide_report_total_and_sex.xlsx
+++ b/Datasets/homicide_report_total_and_sex.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pedroszekely/Documents/GitHub/t2wml/Datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F988301-5408-334C-8EE7-0BD15E6D463A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACB0BDE5-8E7E-2743-8990-2AE5805E6F89}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="30140" windowHeight="17780" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1585,10 +1585,10 @@
     <t>total</t>
   </si>
   <si>
-    <t>------</t>
+    <t>This file has totals by country</t>
   </si>
   <si>
-    <t>This file has totals by country</t>
+    <t>n/a</t>
   </si>
 </sst>
 </file>
@@ -2041,6 +2041,10 @@
     <xf numFmtId="0" fontId="6" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="16" borderId="1" xfId="4" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="11" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2101,10 +2105,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="16" borderId="1" xfId="4" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -2691,28 +2691,28 @@
       <c r="D1" s="25"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B2" s="79" t="s">
+      <c r="B2" s="83" t="s">
         <v>482</v>
       </c>
-      <c r="C2" s="80"/>
-      <c r="D2" s="80"/>
-      <c r="E2" s="80"/>
-      <c r="F2" s="80"/>
-      <c r="G2" s="81"/>
+      <c r="C2" s="84"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="84"/>
+      <c r="F2" s="84"/>
+      <c r="G2" s="85"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B3" s="79" t="s">
+      <c r="B3" s="83" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="81"/>
-      <c r="D3" s="79" t="s">
+      <c r="C3" s="85"/>
+      <c r="D3" s="83" t="s">
         <v>47</v>
       </c>
-      <c r="E3" s="81"/>
-      <c r="F3" s="79" t="s">
+      <c r="E3" s="85"/>
+      <c r="F3" s="83" t="s">
         <v>58</v>
       </c>
-      <c r="G3" s="81"/>
+      <c r="G3" s="85"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="31" t="s">
@@ -2921,34 +2921,34 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B3" s="79" t="s">
+      <c r="B3" s="83" t="s">
         <v>482</v>
       </c>
-      <c r="C3" s="80"/>
-      <c r="D3" s="80"/>
-      <c r="E3" s="80"/>
-      <c r="F3" s="80"/>
-      <c r="G3" s="80"/>
-      <c r="H3" s="80"/>
-      <c r="I3" s="80"/>
-      <c r="J3" s="81"/>
+      <c r="C3" s="84"/>
+      <c r="D3" s="84"/>
+      <c r="E3" s="84"/>
+      <c r="F3" s="84"/>
+      <c r="G3" s="84"/>
+      <c r="H3" s="84"/>
+      <c r="I3" s="84"/>
+      <c r="J3" s="85"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B4" s="79" t="s">
+      <c r="B4" s="83" t="s">
         <v>33</v>
       </c>
-      <c r="C4" s="80"/>
-      <c r="D4" s="81"/>
-      <c r="E4" s="79" t="s">
+      <c r="C4" s="84"/>
+      <c r="D4" s="85"/>
+      <c r="E4" s="83" t="s">
         <v>47</v>
       </c>
-      <c r="F4" s="80"/>
-      <c r="G4" s="81"/>
-      <c r="H4" s="79" t="s">
+      <c r="F4" s="84"/>
+      <c r="G4" s="85"/>
+      <c r="H4" s="83" t="s">
         <v>58</v>
       </c>
-      <c r="I4" s="80"/>
-      <c r="J4" s="81"/>
+      <c r="I4" s="84"/>
+      <c r="J4" s="85"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="31" t="s">
@@ -3108,28 +3108,28 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B3" s="85" t="s">
+      <c r="B3" s="89" t="s">
         <v>482</v>
       </c>
-      <c r="C3" s="85"/>
-      <c r="D3" s="85"/>
-      <c r="E3" s="85"/>
-      <c r="F3" s="85"/>
-      <c r="G3" s="85"/>
+      <c r="C3" s="89"/>
+      <c r="D3" s="89"/>
+      <c r="E3" s="89"/>
+      <c r="F3" s="89"/>
+      <c r="G3" s="89"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B4" s="79" t="s">
+      <c r="B4" s="83" t="s">
         <v>33</v>
       </c>
-      <c r="C4" s="81"/>
-      <c r="D4" s="79" t="s">
+      <c r="C4" s="85"/>
+      <c r="D4" s="83" t="s">
         <v>47</v>
       </c>
-      <c r="E4" s="81"/>
-      <c r="F4" s="85" t="s">
+      <c r="E4" s="85"/>
+      <c r="F4" s="89" t="s">
         <v>58</v>
       </c>
-      <c r="G4" s="85"/>
+      <c r="G4" s="89"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="31" t="s">
@@ -3275,12 +3275,12 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="79" t="s">
+      <c r="A4" s="83" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="80"/>
-      <c r="C4" s="80"/>
-      <c r="D4" s="81"/>
+      <c r="B4" s="84"/>
+      <c r="C4" s="84"/>
+      <c r="D4" s="85"/>
     </row>
     <row r="5" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
@@ -3325,12 +3325,12 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="79" t="s">
+      <c r="A8" s="83" t="s">
         <v>47</v>
       </c>
-      <c r="B8" s="80"/>
-      <c r="C8" s="80"/>
-      <c r="D8" s="81"/>
+      <c r="B8" s="84"/>
+      <c r="C8" s="84"/>
+      <c r="D8" s="85"/>
       <c r="E8">
         <f>B8</f>
         <v>0</v>
@@ -3377,12 +3377,12 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="79" t="s">
+      <c r="A12" s="83" t="s">
         <v>58</v>
       </c>
-      <c r="B12" s="80"/>
-      <c r="C12" s="80"/>
-      <c r="D12" s="81"/>
+      <c r="B12" s="84"/>
+      <c r="C12" s="84"/>
+      <c r="D12" s="85"/>
     </row>
     <row r="13" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
@@ -3470,15 +3470,15 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="79" t="s">
+      <c r="A4" s="83" t="s">
         <v>247</v>
       </c>
-      <c r="B4" s="80"/>
-      <c r="C4" s="80"/>
-      <c r="D4" s="81"/>
+      <c r="B4" s="84"/>
+      <c r="C4" s="84"/>
+      <c r="D4" s="85"/>
     </row>
     <row r="5" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A5" s="86" t="s">
+      <c r="A5" s="90" t="s">
         <v>33</v>
       </c>
       <c r="B5" s="27" t="s">
@@ -3492,7 +3492,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A6" s="87"/>
+      <c r="A6" s="91"/>
       <c r="B6" s="27" t="s">
         <v>275</v>
       </c>
@@ -3504,7 +3504,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A7" s="88"/>
+      <c r="A7" s="92"/>
       <c r="B7" s="27" t="s">
         <v>275</v>
       </c>
@@ -3516,7 +3516,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A8" s="86" t="s">
+      <c r="A8" s="90" t="s">
         <v>47</v>
       </c>
       <c r="B8" s="27" t="s">
@@ -3530,7 +3530,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A9" s="87"/>
+      <c r="A9" s="91"/>
       <c r="B9" s="27" t="s">
         <v>251</v>
       </c>
@@ -3542,7 +3542,7 @@
       </c>
     </row>
     <row r="10" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A10" s="88"/>
+      <c r="A10" s="92"/>
       <c r="B10" s="27" t="s">
         <v>251</v>
       </c>
@@ -3552,7 +3552,7 @@
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A11" s="86" t="s">
+      <c r="A11" s="90" t="s">
         <v>58</v>
       </c>
       <c r="B11" s="27" t="s">
@@ -3566,7 +3566,7 @@
       </c>
     </row>
     <row r="12" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A12" s="87"/>
+      <c r="A12" s="91"/>
       <c r="B12" s="27" t="s">
         <v>251</v>
       </c>
@@ -3578,7 +3578,7 @@
       </c>
     </row>
     <row r="13" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A13" s="88"/>
+      <c r="A13" s="92"/>
       <c r="B13" s="27" t="s">
         <v>251</v>
       </c>
@@ -3590,15 +3590,15 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="79" t="s">
+      <c r="A14" s="83" t="s">
         <v>248</v>
       </c>
-      <c r="B14" s="80"/>
-      <c r="C14" s="80"/>
-      <c r="D14" s="81"/>
+      <c r="B14" s="84"/>
+      <c r="C14" s="84"/>
+      <c r="D14" s="85"/>
     </row>
     <row r="15" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A15" s="86" t="s">
+      <c r="A15" s="90" t="s">
         <v>33</v>
       </c>
       <c r="B15" s="27" t="s">
@@ -3612,7 +3612,7 @@
       </c>
     </row>
     <row r="16" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A16" s="87"/>
+      <c r="A16" s="91"/>
       <c r="B16" s="27" t="s">
         <v>275</v>
       </c>
@@ -3624,7 +3624,7 @@
       </c>
     </row>
     <row r="17" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A17" s="88"/>
+      <c r="A17" s="92"/>
       <c r="B17" s="27" t="s">
         <v>275</v>
       </c>
@@ -3636,7 +3636,7 @@
       </c>
     </row>
     <row r="18" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A18" s="86" t="s">
+      <c r="A18" s="90" t="s">
         <v>47</v>
       </c>
       <c r="B18" s="27" t="s">
@@ -3650,7 +3650,7 @@
       </c>
     </row>
     <row r="19" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A19" s="87"/>
+      <c r="A19" s="91"/>
       <c r="B19" s="27" t="s">
         <v>251</v>
       </c>
@@ -3660,7 +3660,7 @@
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A20" s="88"/>
+      <c r="A20" s="92"/>
       <c r="B20" s="27" t="s">
         <v>251</v>
       </c>
@@ -3672,7 +3672,7 @@
       </c>
     </row>
     <row r="21" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A21" s="86" t="s">
+      <c r="A21" s="90" t="s">
         <v>58</v>
       </c>
       <c r="B21" s="27" t="s">
@@ -3686,7 +3686,7 @@
       </c>
     </row>
     <row r="22" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A22" s="87"/>
+      <c r="A22" s="91"/>
       <c r="B22" s="27" t="s">
         <v>251</v>
       </c>
@@ -3698,7 +3698,7 @@
       </c>
     </row>
     <row r="23" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A23" s="88"/>
+      <c r="A23" s="92"/>
       <c r="B23" s="27" t="s">
         <v>251</v>
       </c>
@@ -3755,12 +3755,12 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="79">
+      <c r="A4" s="83">
         <v>2000</v>
       </c>
-      <c r="B4" s="80"/>
-      <c r="C4" s="80"/>
-      <c r="D4" s="81"/>
+      <c r="B4" s="84"/>
+      <c r="C4" s="84"/>
+      <c r="D4" s="85"/>
     </row>
     <row r="5" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="34" t="s">
@@ -3805,12 +3805,12 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="79">
+      <c r="A8" s="83">
         <v>2001</v>
       </c>
-      <c r="B8" s="80"/>
-      <c r="C8" s="80"/>
-      <c r="D8" s="81"/>
+      <c r="B8" s="84"/>
+      <c r="C8" s="84"/>
+      <c r="D8" s="85"/>
       <c r="F8" t="s">
         <v>502</v>
       </c>
@@ -3870,12 +3870,12 @@
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="79">
+      <c r="A12" s="83">
         <v>2002</v>
       </c>
-      <c r="B12" s="80"/>
-      <c r="C12" s="80"/>
-      <c r="D12" s="81"/>
+      <c r="B12" s="84"/>
+      <c r="C12" s="84"/>
+      <c r="D12" s="85"/>
     </row>
     <row r="13" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="34" t="s">
@@ -4154,12 +4154,12 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="73">
+      <c r="A4" s="77">
         <v>2000</v>
       </c>
-      <c r="B4" s="74"/>
-      <c r="C4" s="74"/>
-      <c r="D4" s="75"/>
+      <c r="B4" s="78"/>
+      <c r="C4" s="78"/>
+      <c r="D4" s="79"/>
     </row>
     <row r="5" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="61" t="s">
@@ -4240,12 +4240,12 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="73">
+      <c r="A11" s="77">
         <v>2001</v>
       </c>
-      <c r="B11" s="74"/>
-      <c r="C11" s="74"/>
-      <c r="D11" s="75"/>
+      <c r="B11" s="78"/>
+      <c r="C11" s="78"/>
+      <c r="D11" s="79"/>
     </row>
     <row r="12" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="61" t="s">
@@ -4326,12 +4326,12 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="73">
+      <c r="A18" s="77">
         <v>2002</v>
       </c>
-      <c r="B18" s="74"/>
-      <c r="C18" s="74"/>
-      <c r="D18" s="75"/>
+      <c r="B18" s="78"/>
+      <c r="C18" s="78"/>
+      <c r="D18" s="79"/>
     </row>
     <row r="19" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="61" t="s">
@@ -4972,7 +4972,7 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5068,7 +5068,7 @@
       <c r="B6" s="48" t="s">
         <v>275</v>
       </c>
-      <c r="C6" s="93" t="s">
+      <c r="C6" s="73" t="s">
         <v>479</v>
       </c>
       <c r="D6" s="26">
@@ -5097,8 +5097,8 @@
       <c r="E7" s="46">
         <v>1</v>
       </c>
-      <c r="F7" s="96" t="s">
-        <v>509</v>
+      <c r="F7" s="76" t="s">
+        <v>510</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -5114,8 +5114,8 @@
       <c r="D8" s="46">
         <v>4</v>
       </c>
-      <c r="E8" s="96" t="s">
-        <v>509</v>
+      <c r="E8" s="76" t="s">
+        <v>510</v>
       </c>
       <c r="F8" s="46">
         <v>8</v>
@@ -5128,7 +5128,7 @@
       <c r="B9" s="48" t="s">
         <v>251</v>
       </c>
-      <c r="C9" s="93" t="s">
+      <c r="C9" s="73" t="s">
         <v>479</v>
       </c>
       <c r="D9" s="26">
@@ -5177,8 +5177,8 @@
       <c r="E11" s="46">
         <v>1</v>
       </c>
-      <c r="F11" s="96" t="s">
-        <v>509</v>
+      <c r="F11" s="76" t="s">
+        <v>510</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -5188,7 +5188,7 @@
       <c r="B12" s="48" t="s">
         <v>251</v>
       </c>
-      <c r="C12" s="93" t="s">
+      <c r="C12" s="73" t="s">
         <v>479</v>
       </c>
       <c r="D12" s="26">
@@ -5202,12 +5202,12 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A13" s="95" t="s">
-        <v>510</v>
+      <c r="A13" s="75" t="s">
+        <v>509</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B16" s="94"/>
+      <c r="B16" s="74"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5276,23 +5276,23 @@
       <c r="A3" s="18" t="s">
         <v>419</v>
       </c>
-      <c r="B3" s="89" t="s">
+      <c r="B3" s="93" t="s">
         <v>421</v>
       </c>
-      <c r="C3" s="89"/>
-      <c r="D3" s="89"/>
-      <c r="E3" s="89"/>
-      <c r="F3" s="89"/>
-      <c r="G3" s="89"/>
-      <c r="H3" s="89"/>
-      <c r="I3" s="89"/>
-      <c r="J3" s="89"/>
-      <c r="K3" s="89"/>
-      <c r="L3" s="89"/>
-      <c r="M3" s="89"/>
-      <c r="N3" s="89"/>
-      <c r="O3" s="89"/>
-      <c r="P3" s="89"/>
+      <c r="C3" s="93"/>
+      <c r="D3" s="93"/>
+      <c r="E3" s="93"/>
+      <c r="F3" s="93"/>
+      <c r="G3" s="93"/>
+      <c r="H3" s="93"/>
+      <c r="I3" s="93"/>
+      <c r="J3" s="93"/>
+      <c r="K3" s="93"/>
+      <c r="L3" s="93"/>
+      <c r="M3" s="93"/>
+      <c r="N3" s="93"/>
+      <c r="O3" s="93"/>
+      <c r="P3" s="93"/>
     </row>
     <row r="4" spans="1:39" s="21" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="18"/>
@@ -5313,44 +5313,44 @@
       <c r="P4" s="22"/>
     </row>
     <row r="5" spans="1:39" x14ac:dyDescent="0.2">
-      <c r="E5" s="90" t="s">
+      <c r="E5" s="94" t="s">
         <v>422</v>
       </c>
-      <c r="F5" s="91"/>
-      <c r="G5" s="91"/>
-      <c r="H5" s="91"/>
-      <c r="I5" s="91"/>
-      <c r="J5" s="91"/>
-      <c r="K5" s="91"/>
-      <c r="L5" s="91"/>
-      <c r="M5" s="91"/>
-      <c r="N5" s="91"/>
-      <c r="O5" s="91"/>
-      <c r="P5" s="91"/>
-      <c r="Q5" s="91"/>
-      <c r="R5" s="91"/>
-      <c r="S5" s="91"/>
-      <c r="T5" s="91"/>
-      <c r="U5" s="92"/>
-      <c r="W5" s="90" t="s">
+      <c r="F5" s="95"/>
+      <c r="G5" s="95"/>
+      <c r="H5" s="95"/>
+      <c r="I5" s="95"/>
+      <c r="J5" s="95"/>
+      <c r="K5" s="95"/>
+      <c r="L5" s="95"/>
+      <c r="M5" s="95"/>
+      <c r="N5" s="95"/>
+      <c r="O5" s="95"/>
+      <c r="P5" s="95"/>
+      <c r="Q5" s="95"/>
+      <c r="R5" s="95"/>
+      <c r="S5" s="95"/>
+      <c r="T5" s="95"/>
+      <c r="U5" s="96"/>
+      <c r="W5" s="94" t="s">
         <v>423</v>
       </c>
-      <c r="X5" s="91"/>
-      <c r="Y5" s="91"/>
-      <c r="Z5" s="91"/>
-      <c r="AA5" s="91"/>
-      <c r="AB5" s="91"/>
-      <c r="AC5" s="91"/>
-      <c r="AD5" s="91"/>
-      <c r="AE5" s="91"/>
-      <c r="AF5" s="91"/>
-      <c r="AG5" s="91"/>
-      <c r="AH5" s="91"/>
-      <c r="AI5" s="91"/>
-      <c r="AJ5" s="91"/>
-      <c r="AK5" s="91"/>
-      <c r="AL5" s="91"/>
-      <c r="AM5" s="92"/>
+      <c r="X5" s="95"/>
+      <c r="Y5" s="95"/>
+      <c r="Z5" s="95"/>
+      <c r="AA5" s="95"/>
+      <c r="AB5" s="95"/>
+      <c r="AC5" s="95"/>
+      <c r="AD5" s="95"/>
+      <c r="AE5" s="95"/>
+      <c r="AF5" s="95"/>
+      <c r="AG5" s="95"/>
+      <c r="AH5" s="95"/>
+      <c r="AI5" s="95"/>
+      <c r="AJ5" s="95"/>
+      <c r="AK5" s="95"/>
+      <c r="AL5" s="95"/>
+      <c r="AM5" s="96"/>
     </row>
     <row r="6" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
@@ -27360,23 +27360,23 @@
       <c r="A3" s="18" t="s">
         <v>419</v>
       </c>
-      <c r="B3" s="89" t="s">
+      <c r="B3" s="93" t="s">
         <v>421</v>
       </c>
-      <c r="C3" s="89"/>
-      <c r="D3" s="89"/>
-      <c r="E3" s="89"/>
-      <c r="F3" s="89"/>
-      <c r="G3" s="89"/>
-      <c r="H3" s="89"/>
-      <c r="I3" s="89"/>
-      <c r="J3" s="89"/>
-      <c r="K3" s="89"/>
-      <c r="L3" s="89"/>
-      <c r="M3" s="89"/>
-      <c r="N3" s="89"/>
-      <c r="O3" s="89"/>
-      <c r="P3" s="89"/>
+      <c r="C3" s="93"/>
+      <c r="D3" s="93"/>
+      <c r="E3" s="93"/>
+      <c r="F3" s="93"/>
+      <c r="G3" s="93"/>
+      <c r="H3" s="93"/>
+      <c r="I3" s="93"/>
+      <c r="J3" s="93"/>
+      <c r="K3" s="93"/>
+      <c r="L3" s="93"/>
+      <c r="M3" s="93"/>
+      <c r="N3" s="93"/>
+      <c r="O3" s="93"/>
+      <c r="P3" s="93"/>
     </row>
     <row r="4" spans="1:40" s="21" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="18"/>
@@ -27397,44 +27397,44 @@
       <c r="P4" s="22"/>
     </row>
     <row r="5" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="F5" s="90" t="s">
+      <c r="F5" s="94" t="s">
         <v>424</v>
       </c>
-      <c r="G5" s="91"/>
-      <c r="H5" s="91"/>
-      <c r="I5" s="91"/>
-      <c r="J5" s="91"/>
-      <c r="K5" s="91"/>
-      <c r="L5" s="91"/>
-      <c r="M5" s="91"/>
-      <c r="N5" s="91"/>
-      <c r="O5" s="91"/>
-      <c r="P5" s="91"/>
-      <c r="Q5" s="91"/>
-      <c r="R5" s="91"/>
-      <c r="S5" s="91"/>
-      <c r="T5" s="91"/>
-      <c r="U5" s="91"/>
-      <c r="V5" s="92"/>
-      <c r="X5" s="90" t="s">
+      <c r="G5" s="95"/>
+      <c r="H5" s="95"/>
+      <c r="I5" s="95"/>
+      <c r="J5" s="95"/>
+      <c r="K5" s="95"/>
+      <c r="L5" s="95"/>
+      <c r="M5" s="95"/>
+      <c r="N5" s="95"/>
+      <c r="O5" s="95"/>
+      <c r="P5" s="95"/>
+      <c r="Q5" s="95"/>
+      <c r="R5" s="95"/>
+      <c r="S5" s="95"/>
+      <c r="T5" s="95"/>
+      <c r="U5" s="95"/>
+      <c r="V5" s="96"/>
+      <c r="X5" s="94" t="s">
         <v>425</v>
       </c>
-      <c r="Y5" s="91"/>
-      <c r="Z5" s="91"/>
-      <c r="AA5" s="91"/>
-      <c r="AB5" s="91"/>
-      <c r="AC5" s="91"/>
-      <c r="AD5" s="91"/>
-      <c r="AE5" s="91"/>
-      <c r="AF5" s="91"/>
-      <c r="AG5" s="91"/>
-      <c r="AH5" s="91"/>
-      <c r="AI5" s="91"/>
-      <c r="AJ5" s="91"/>
-      <c r="AK5" s="91"/>
-      <c r="AL5" s="91"/>
-      <c r="AM5" s="91"/>
-      <c r="AN5" s="92"/>
+      <c r="Y5" s="95"/>
+      <c r="Z5" s="95"/>
+      <c r="AA5" s="95"/>
+      <c r="AB5" s="95"/>
+      <c r="AC5" s="95"/>
+      <c r="AD5" s="95"/>
+      <c r="AE5" s="95"/>
+      <c r="AF5" s="95"/>
+      <c r="AG5" s="95"/>
+      <c r="AH5" s="95"/>
+      <c r="AI5" s="95"/>
+      <c r="AJ5" s="95"/>
+      <c r="AK5" s="95"/>
+      <c r="AL5" s="95"/>
+      <c r="AM5" s="95"/>
+      <c r="AN5" s="96"/>
     </row>
     <row r="6" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
@@ -63722,16 +63722,16 @@
       <c r="B3" s="49" t="s">
         <v>249</v>
       </c>
-      <c r="C3" s="73" t="s">
+      <c r="C3" s="77" t="s">
         <v>248</v>
       </c>
-      <c r="D3" s="74"/>
-      <c r="E3" s="75"/>
-      <c r="F3" s="76" t="s">
+      <c r="D3" s="78"/>
+      <c r="E3" s="79"/>
+      <c r="F3" s="80" t="s">
         <v>247</v>
       </c>
-      <c r="G3" s="77"/>
-      <c r="H3" s="78"/>
+      <c r="G3" s="81"/>
+      <c r="H3" s="82"/>
     </row>
     <row r="4" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="68"/>
@@ -63877,16 +63877,16 @@
     <row r="4" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="27"/>
       <c r="B4" s="27"/>
-      <c r="C4" s="79" t="s">
+      <c r="C4" s="83" t="s">
         <v>248</v>
       </c>
-      <c r="D4" s="80"/>
-      <c r="E4" s="81"/>
-      <c r="F4" s="82" t="s">
+      <c r="D4" s="84"/>
+      <c r="E4" s="85"/>
+      <c r="F4" s="86" t="s">
         <v>247</v>
       </c>
-      <c r="G4" s="83"/>
-      <c r="H4" s="84"/>
+      <c r="G4" s="87"/>
+      <c r="H4" s="88"/>
     </row>
     <row r="5" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="27" t="s">
@@ -63994,18 +63994,18 @@
       <c r="B2" s="25"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="C3" s="82">
+      <c r="C3" s="86">
         <v>2000</v>
       </c>
-      <c r="D3" s="84"/>
-      <c r="E3" s="82">
+      <c r="D3" s="88"/>
+      <c r="E3" s="86">
         <v>2001</v>
       </c>
-      <c r="F3" s="84"/>
-      <c r="G3" s="82">
+      <c r="F3" s="88"/>
+      <c r="G3" s="86">
         <v>2002</v>
       </c>
-      <c r="H3" s="84"/>
+      <c r="H3" s="88"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="29" t="s">
@@ -64159,18 +64159,18 @@
       <c r="B2" s="66"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C3" s="76">
+      <c r="C3" s="80">
         <v>2000</v>
       </c>
-      <c r="D3" s="78"/>
-      <c r="E3" s="76">
+      <c r="D3" s="82"/>
+      <c r="E3" s="80">
         <v>2001</v>
       </c>
-      <c r="F3" s="78"/>
-      <c r="G3" s="76">
+      <c r="F3" s="82"/>
+      <c r="G3" s="80">
         <v>2002</v>
       </c>
-      <c r="H3" s="78"/>
+      <c r="H3" s="82"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="49" t="s">
@@ -64336,28 +64336,28 @@
       <c r="D1" s="25"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C2" s="79" t="s">
+      <c r="C2" s="83" t="s">
         <v>482</v>
       </c>
-      <c r="D2" s="80"/>
-      <c r="E2" s="80"/>
-      <c r="F2" s="80"/>
-      <c r="G2" s="80"/>
-      <c r="H2" s="81"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="84"/>
+      <c r="F2" s="84"/>
+      <c r="G2" s="84"/>
+      <c r="H2" s="85"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C3" s="79" t="s">
+      <c r="C3" s="83" t="s">
         <v>33</v>
       </c>
-      <c r="D3" s="81"/>
-      <c r="E3" s="79" t="s">
+      <c r="D3" s="85"/>
+      <c r="E3" s="83" t="s">
         <v>47</v>
       </c>
-      <c r="F3" s="81"/>
-      <c r="G3" s="79" t="s">
+      <c r="F3" s="85"/>
+      <c r="G3" s="83" t="s">
         <v>58</v>
       </c>
-      <c r="H3" s="81"/>
+      <c r="H3" s="85"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="31" t="s">

</xml_diff>

<commit_message>
Update examples for the paper
</commit_message>
<xml_diff>
--- a/Datasets/homicide_report_total_and_sex.xlsx
+++ b/Datasets/homicide_report_total_and_sex.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10715"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pedroszekely/Documents/GitHub/t2wml/Datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACB0BDE5-8E7E-2743-8990-2AE5805E6F89}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F78D6477-195A-BF4C-9FB2-5AC9D328C4E9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="30140" windowHeight="17780" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3825" uniqueCount="511">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3826" uniqueCount="512">
   <si>
     <t>UNODC Name</t>
   </si>
@@ -1590,6 +1590,9 @@
   <si>
     <t>n/a</t>
   </si>
+  <si>
+    <t>Highlights by Pedro</t>
+  </si>
 </sst>
 </file>
 
@@ -1949,7 +1952,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="97">
+  <cellXfs count="98">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -2105,6 +2108,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="3" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -4969,10 +4973,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{306E606D-CC25-7440-B1DE-7CB61853CD87}">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4996,49 +5000,37 @@
       <c r="F1" s="25"/>
     </row>
     <row r="2" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" s="25"/>
-      <c r="B2" s="25"/>
+      <c r="A2" s="18"/>
+      <c r="B2" s="19"/>
       <c r="C2" s="25"/>
       <c r="D2" s="25"/>
       <c r="E2" s="25"/>
       <c r="F2" s="25"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="49" t="s">
+    <row r="3" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="25"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="49" t="s">
+      <c r="B4" s="49" t="s">
         <v>249</v>
       </c>
-      <c r="C3" s="49"/>
-      <c r="D3" s="47">
+      <c r="C4" s="49"/>
+      <c r="D4" s="47">
         <v>2000</v>
       </c>
-      <c r="E3" s="47">
+      <c r="E4" s="47">
         <v>2001</v>
       </c>
-      <c r="F3" s="47">
+      <c r="F4" s="47">
         <v>2002</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A4" s="48" t="s">
-        <v>33</v>
-      </c>
-      <c r="B4" s="48" t="s">
-        <v>275</v>
-      </c>
-      <c r="C4" s="48" t="s">
-        <v>247</v>
-      </c>
-      <c r="D4" s="46">
-        <v>1</v>
-      </c>
-      <c r="E4" s="46">
-        <v>2</v>
-      </c>
-      <c r="F4" s="46">
-        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -5049,16 +5041,16 @@
         <v>275</v>
       </c>
       <c r="C5" s="48" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D5" s="46">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E5" s="46">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F5" s="46">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -5068,37 +5060,37 @@
       <c r="B6" s="48" t="s">
         <v>275</v>
       </c>
-      <c r="C6" s="73" t="s">
-        <v>479</v>
-      </c>
-      <c r="D6" s="26">
+      <c r="C6" s="48" t="s">
+        <v>248</v>
+      </c>
+      <c r="D6" s="46">
+        <v>4</v>
+      </c>
+      <c r="E6" s="46">
         <v>5</v>
       </c>
-      <c r="E6" s="26">
-        <v>7</v>
-      </c>
-      <c r="F6" s="26">
-        <v>8</v>
+      <c r="F6" s="46">
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="48" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="B7" s="48" t="s">
-        <v>251</v>
-      </c>
-      <c r="C7" s="48" t="s">
-        <v>247</v>
-      </c>
-      <c r="D7" s="46">
-        <v>2</v>
-      </c>
-      <c r="E7" s="46">
-        <v>1</v>
-      </c>
-      <c r="F7" s="76" t="s">
-        <v>510</v>
+        <v>275</v>
+      </c>
+      <c r="C7" s="73" t="s">
+        <v>479</v>
+      </c>
+      <c r="D7" s="26">
+        <v>5</v>
+      </c>
+      <c r="E7" s="26">
+        <v>7</v>
+      </c>
+      <c r="F7" s="26">
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -5109,16 +5101,16 @@
         <v>251</v>
       </c>
       <c r="C8" s="48" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D8" s="46">
-        <v>4</v>
-      </c>
-      <c r="E8" s="76" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" s="46">
+        <v>1</v>
+      </c>
+      <c r="F8" s="76" t="s">
         <v>510</v>
-      </c>
-      <c r="F8" s="46">
-        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -5128,37 +5120,37 @@
       <c r="B9" s="48" t="s">
         <v>251</v>
       </c>
-      <c r="C9" s="73" t="s">
-        <v>479</v>
-      </c>
-      <c r="D9" s="26">
-        <v>6</v>
-      </c>
-      <c r="E9" s="26">
-        <v>1</v>
-      </c>
-      <c r="F9" s="26">
+      <c r="C9" s="48" t="s">
+        <v>248</v>
+      </c>
+      <c r="D9" s="46">
+        <v>4</v>
+      </c>
+      <c r="E9" s="76" t="s">
+        <v>510</v>
+      </c>
+      <c r="F9" s="46">
         <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="48" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="B10" s="48" t="s">
         <v>251</v>
       </c>
-      <c r="C10" s="48" t="s">
-        <v>247</v>
-      </c>
-      <c r="D10" s="46">
-        <v>2</v>
-      </c>
-      <c r="E10" s="46">
+      <c r="C10" s="73" t="s">
+        <v>479</v>
+      </c>
+      <c r="D10" s="26">
+        <v>6</v>
+      </c>
+      <c r="E10" s="26">
         <v>1</v>
       </c>
-      <c r="F10" s="46">
-        <v>3</v>
+      <c r="F10" s="26">
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -5169,16 +5161,16 @@
         <v>251</v>
       </c>
       <c r="C11" s="48" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D11" s="46">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E11" s="46">
         <v>1</v>
       </c>
-      <c r="F11" s="76" t="s">
-        <v>510</v>
+      <c r="F11" s="46">
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -5188,26 +5180,51 @@
       <c r="B12" s="48" t="s">
         <v>251</v>
       </c>
-      <c r="C12" s="73" t="s">
+      <c r="C12" s="48" t="s">
+        <v>248</v>
+      </c>
+      <c r="D12" s="46">
+        <v>1</v>
+      </c>
+      <c r="E12" s="46">
+        <v>1</v>
+      </c>
+      <c r="F12" s="76" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A13" s="48" t="s">
+        <v>58</v>
+      </c>
+      <c r="B13" s="48" t="s">
+        <v>251</v>
+      </c>
+      <c r="C13" s="73" t="s">
         <v>479</v>
       </c>
-      <c r="D12" s="26">
+      <c r="D13" s="26">
         <v>3</v>
       </c>
-      <c r="E12" s="26">
+      <c r="E13" s="26">
         <v>2</v>
       </c>
-      <c r="F12" s="26">
+      <c r="F13" s="26">
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A13" s="75" t="s">
+    <row r="14" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A14" s="75" t="s">
         <v>509</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B16" s="74"/>
+    <row r="15" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A15" s="97" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B17" s="74"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
generalized datetime parser module
</commit_message>
<xml_diff>
--- a/Datasets/homicide_report_total_and_sex.xlsx
+++ b/Datasets/homicide_report_total_and_sex.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\isi\T2WML\t2wml\Datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3117D1D-F5F7-4FEB-AD0B-18BA0A5C236A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7510F0E3-D663-4675-B0BB-048EB926F260}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2396,7 +2396,7 @@
   <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.77734375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -4978,7 +4978,7 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>